<commit_message>
Removed viscosity temperature scaling and loosened a3 constraints
</commit_message>
<xml_diff>
--- a/turbineData.xlsx
+++ b/turbineData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ellio\OneDrive\Documents\Fall 2025 Classes\AE4453\HW4\turbineDesigner\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ellio\OneDrive\Documents\Fall 2025 Classes\AE4453\HW4\turbineDesigner\turbineDesigner-main\turbineDesigner-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30714C9F-1100-48EA-8A81-1F38A9371AAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2C34D16-A9AE-40EB-BB30-832B8528A19A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -493,18 +493,18 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="7.7265625" customWidth="1"/>
-    <col min="2" max="2" width="13.453125" customWidth="1"/>
+    <col min="2" max="2" width="12.453125" customWidth="1"/>
     <col min="3" max="3" width="11.453125" customWidth="1"/>
     <col min="4" max="5" width="12.453125" customWidth="1"/>
     <col min="6" max="6" width="12.08984375" customWidth="1"/>
-    <col min="7" max="8" width="12.453125" customWidth="1"/>
-    <col min="9" max="9" width="11.453125" customWidth="1"/>
+    <col min="7" max="7" width="12.453125" customWidth="1"/>
+    <col min="8" max="9" width="11.453125" customWidth="1"/>
     <col min="10" max="10" width="13.453125" customWidth="1"/>
     <col min="11" max="12" width="12.453125" customWidth="1"/>
     <col min="13" max="13" width="17" customWidth="1"/>
@@ -544,34 +544,34 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B2">
-        <v>5.258880384056687E-2</v>
+        <v>0.13409993242852528</v>
       </c>
       <c r="C2">
-        <v>335.81294277237402</v>
+        <v>288.25533153052328</v>
       </c>
       <c r="D2">
-        <v>0.40489613482165981</v>
+        <v>0.34755500670966555</v>
       </c>
       <c r="E2">
-        <v>0.85762030975445958</v>
+        <v>0.99911421749194518</v>
       </c>
       <c r="F2">
-        <v>-2.4746512740451219</v>
+        <v>-3.3585681937866774</v>
       </c>
       <c r="G2">
         <v>1692.680036512749</v>
       </c>
       <c r="H2">
-        <v>715.72063412245154</v>
+        <v>716.50780749594855</v>
       </c>
       <c r="I2">
-        <v>91.391485105315823</v>
+        <v>91.550599021366125</v>
       </c>
       <c r="J2">
-        <v>91.890210822098638</v>
+        <v>92.040123781531463</v>
       </c>
       <c r="K2">
-        <v>0.61774742972448016</v>
+        <v>0.59592219376540101</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
@@ -620,25 +620,25 @@
         <v>1.1122378174840659</v>
       </c>
       <c r="E4">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="F4">
-        <v>149000.00031017588</v>
+        <v>149000.0005574617</v>
       </c>
       <c r="G4">
-        <v>0.38898352951184534</v>
+        <v>0.32887959639802616</v>
       </c>
       <c r="H4">
-        <v>0.42020658461707477</v>
+        <v>0.36527684904874924</v>
       </c>
       <c r="I4">
-        <v>1.1586267142476763</v>
+        <v>1.3936395955527214</v>
       </c>
       <c r="J4">
-        <v>5.0712933160485661E-2</v>
+        <v>4.852687173693504E-2</v>
       </c>
       <c r="K4">
-        <v>0.96600002296613974</v>
+        <v>0.96752073569314956</v>
       </c>
       <c r="L4">
         <v>0.35677943421965702</v>
@@ -687,43 +687,43 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>-56.381415949168129</v>
+        <v>-61.146699297271851</v>
       </c>
       <c r="B6">
-        <v>-63.334720033024318</v>
+        <v>-69.803054086655365</v>
       </c>
       <c r="C6">
-        <v>-18.677578169850719</v>
+        <v>-39.149212752582415</v>
       </c>
       <c r="D6">
-        <v>1.986123692843405</v>
+        <v>1.7077055259324219</v>
       </c>
       <c r="E6">
-        <v>133</v>
+        <v>113</v>
       </c>
       <c r="F6">
-        <v>113000.00131316822</v>
+        <v>113000.0023600851</v>
       </c>
       <c r="G6">
-        <v>0.37994290569517891</v>
+        <v>0.31818390295631632</v>
       </c>
       <c r="H6">
-        <v>0.42839835246992236</v>
+        <v>0.37463044360729258</v>
       </c>
       <c r="I6">
-        <v>1.2754529766190168</v>
+        <v>1.7104066382790681</v>
       </c>
       <c r="J6">
-        <v>6.4451704888049105E-2</v>
+        <v>5.035868318259603E-2</v>
       </c>
       <c r="K6">
-        <v>0.57301748794397911</v>
+        <v>0.57274607373599251</v>
       </c>
       <c r="L6">
-        <v>0.62315607015416108</v>
+        <v>0.67296415604893989</v>
       </c>
       <c r="M6">
-        <v>7718583.0979606612</v>
+        <v>7706451.3191588884</v>
       </c>
     </row>
   </sheetData>

</xml_diff>